<commit_message>
Update biomass calculators and map year headings
</commit_message>
<xml_diff>
--- a/server/biomassStock/calculator_boreal_en.xlsx
+++ b/server/biomassStock/calculator_boreal_en.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="21570" windowHeight="7560"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="21570" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="9" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="83">
   <si>
     <t>1000 ha</t>
   </si>
@@ -307,9 +307,6 @@
     <t xml:space="preserve"> % of Growing stock</t>
   </si>
   <si>
-    <t>In Sections 1 and 2 you insert data from reporting tables 1b and 2a, and in Section 3  you insert the estimated  percentages of growing stock by combination of FRA forest type and IPCC forest type. Once you are done, copy sections 3 to 6 and paste them in the comment section below table 2c in the FRA platform. Finally, copy the data from Section 7 to table 2c in the platform and data from Section 8 to table 2d in the platform</t>
-  </si>
-  <si>
     <t>Input data on Forest area from  reporting table 1b</t>
   </si>
   <si>
@@ -323,6 +320,15 @@
   </si>
   <si>
     <t>Copy highlighted carbon values into FRA platform table 2d</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>In Sections 1 and 2 you insert data from reporting tables 1b and 2a, and in Section 3  you insert the estimated  percentages of growing stock by combination of FRA forest type and IPCC forest type. Once you are done, copy sections 3 to 8 and paste them in the comment section below table 2c in the FRA platform. Finally, copy the data from Section 9 to table 2c in the platform and data from Section 10 to table 2d in the platform.</t>
   </si>
 </sst>
 </file>
@@ -1295,17 +1301,17 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1648,7 +1654,7 @@
   <dimension ref="B1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1693,7 +1699,7 @@
         <v>66</v>
       </c>
       <c r="F3" s="41">
-        <v>43025</v>
+        <v>43084</v>
       </c>
       <c r="G3" s="80"/>
       <c r="H3" s="81"/>
@@ -1721,18 +1727,18 @@
       <c r="B5" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="122" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="122"/>
-      <c r="E5" s="122"/>
-      <c r="F5" s="122"/>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
-      <c r="J5" s="122"/>
-      <c r="K5" s="122"/>
-      <c r="L5" s="122"/>
+      <c r="C5" s="125" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
       <c r="M5" s="37"/>
     </row>
     <row r="6" spans="2:23" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1843,7 +1849,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
@@ -2198,7 +2204,7 @@
         <v>32</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
@@ -2438,7 +2444,7 @@
       <c r="B35" s="34"/>
       <c r="C35" s="36"/>
       <c r="D35" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
@@ -3028,15 +3034,15 @@
       <c r="C61" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="D61" s="123"/>
-      <c r="E61" s="124"/>
-      <c r="F61" s="124"/>
-      <c r="G61" s="124"/>
-      <c r="H61" s="124"/>
-      <c r="I61" s="124"/>
-      <c r="J61" s="124"/>
-      <c r="K61" s="124"/>
-      <c r="L61" s="125"/>
+      <c r="D61" s="122"/>
+      <c r="E61" s="123"/>
+      <c r="F61" s="123"/>
+      <c r="G61" s="123"/>
+      <c r="H61" s="123"/>
+      <c r="I61" s="123"/>
+      <c r="J61" s="123"/>
+      <c r="K61" s="123"/>
+      <c r="L61" s="124"/>
       <c r="M61" s="66"/>
       <c r="N61" s="66"/>
     </row>
@@ -3221,15 +3227,15 @@
       <c r="C66" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="123"/>
-      <c r="E66" s="124"/>
-      <c r="F66" s="124"/>
-      <c r="G66" s="124"/>
-      <c r="H66" s="124"/>
-      <c r="I66" s="124"/>
-      <c r="J66" s="124"/>
-      <c r="K66" s="124"/>
-      <c r="L66" s="125"/>
+      <c r="D66" s="122"/>
+      <c r="E66" s="123"/>
+      <c r="F66" s="123"/>
+      <c r="G66" s="123"/>
+      <c r="H66" s="123"/>
+      <c r="I66" s="123"/>
+      <c r="J66" s="123"/>
+      <c r="K66" s="123"/>
+      <c r="L66" s="124"/>
       <c r="M66" s="66"/>
       <c r="N66" s="66"/>
     </row>
@@ -3414,15 +3420,15 @@
       <c r="C71" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="123"/>
-      <c r="E71" s="124"/>
-      <c r="F71" s="124"/>
-      <c r="G71" s="124"/>
-      <c r="H71" s="124"/>
-      <c r="I71" s="124"/>
-      <c r="J71" s="124"/>
-      <c r="K71" s="124"/>
-      <c r="L71" s="125"/>
+      <c r="D71" s="122"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="123"/>
+      <c r="G71" s="123"/>
+      <c r="H71" s="123"/>
+      <c r="I71" s="123"/>
+      <c r="J71" s="123"/>
+      <c r="K71" s="123"/>
+      <c r="L71" s="124"/>
       <c r="M71" s="66"/>
       <c r="N71" s="66"/>
     </row>
@@ -3590,7 +3596,7 @@
     </row>
     <row r="77" spans="2:14" s="51" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="87" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C77" s="93" t="s">
         <v>50</v>
@@ -3838,15 +3844,15 @@
       <c r="C84" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="D84" s="123"/>
-      <c r="E84" s="124"/>
-      <c r="F84" s="124"/>
-      <c r="G84" s="124"/>
-      <c r="H84" s="124"/>
-      <c r="I84" s="124"/>
-      <c r="J84" s="124"/>
-      <c r="K84" s="124"/>
-      <c r="L84" s="125"/>
+      <c r="D84" s="122"/>
+      <c r="E84" s="123"/>
+      <c r="F84" s="123"/>
+      <c r="G84" s="123"/>
+      <c r="H84" s="123"/>
+      <c r="I84" s="123"/>
+      <c r="J84" s="123"/>
+      <c r="K84" s="123"/>
+      <c r="L84" s="124"/>
       <c r="M84" s="66"/>
       <c r="N84" s="66"/>
     </row>
@@ -4031,15 +4037,15 @@
       <c r="C89" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D89" s="123"/>
-      <c r="E89" s="124"/>
-      <c r="F89" s="124"/>
-      <c r="G89" s="124"/>
-      <c r="H89" s="124"/>
-      <c r="I89" s="124"/>
-      <c r="J89" s="124"/>
-      <c r="K89" s="124"/>
-      <c r="L89" s="125"/>
+      <c r="D89" s="122"/>
+      <c r="E89" s="123"/>
+      <c r="F89" s="123"/>
+      <c r="G89" s="123"/>
+      <c r="H89" s="123"/>
+      <c r="I89" s="123"/>
+      <c r="J89" s="123"/>
+      <c r="K89" s="123"/>
+      <c r="L89" s="124"/>
       <c r="M89" s="66"/>
       <c r="N89" s="66"/>
     </row>
@@ -4224,15 +4230,15 @@
       <c r="C94" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="D94" s="123"/>
-      <c r="E94" s="124"/>
-      <c r="F94" s="124"/>
-      <c r="G94" s="124"/>
-      <c r="H94" s="124"/>
-      <c r="I94" s="124"/>
-      <c r="J94" s="124"/>
-      <c r="K94" s="124"/>
-      <c r="L94" s="125"/>
+      <c r="D94" s="122"/>
+      <c r="E94" s="123"/>
+      <c r="F94" s="123"/>
+      <c r="G94" s="123"/>
+      <c r="H94" s="123"/>
+      <c r="I94" s="123"/>
+      <c r="J94" s="123"/>
+      <c r="K94" s="123"/>
+      <c r="L94" s="124"/>
       <c r="M94" s="66"/>
       <c r="N94" s="66"/>
     </row>
@@ -4400,7 +4406,7 @@
     </row>
     <row r="100" spans="2:14" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B100" s="87" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C100" s="93" t="s">
         <v>56</v>
@@ -4673,7 +4679,7 @@
     </row>
     <row r="109" spans="2:14" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B109" s="87" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C109" s="93" t="s">
         <v>59</v>
@@ -4976,10 +4982,10 @@
     </row>
     <row r="120" spans="2:14" s="51" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="58" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C120" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N120" s="52"/>
     </row>
@@ -5158,10 +5164,10 @@
     </row>
     <row r="128" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="58" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C128" s="49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D128" s="76"/>
       <c r="E128" s="76"/>
@@ -5845,13 +5851,8 @@
       <c r="M168" s="76"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zaZWvD/YT8nA47E1s1PPkYqVpYBjDOwp5Pdxnz+w4EqwWm97uiQZMwMhcOoBXdh/YfMKkN4C30HU5LPrJwqZsQ==" saltValue="mjvvZowgl58KmE4qAeFkrg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="o+oQNtlV04+KJUG005s2Eb3VRI3RhKd1OsOf9KuMM/yTGMGY9s+otfbV2dgiamNGC5nvuCGCUViicd9es8nHtw==" saltValue="VRIFU3I/1JZPq0F6TXwuAg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="D66:L66"/>
-    <mergeCell ref="D84:L84"/>
-    <mergeCell ref="D89:L89"/>
-    <mergeCell ref="D71:L71"/>
-    <mergeCell ref="D94:L94"/>
     <mergeCell ref="C5:L5"/>
     <mergeCell ref="D61:L61"/>
     <mergeCell ref="F6:G6"/>
@@ -5867,6 +5868,11 @@
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D66:L66"/>
+    <mergeCell ref="D84:L84"/>
+    <mergeCell ref="D89:L89"/>
+    <mergeCell ref="D71:L71"/>
+    <mergeCell ref="D94:L94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated biomass calculator in en and es
</commit_message>
<xml_diff>
--- a/server/biomassStock/calculator_boreal_en.xlsx
+++ b/server/biomassStock/calculator_boreal_en.xlsx
@@ -313,9 +313,6 @@
     <t>Input data on Growing stock from  reporting table 2a</t>
   </si>
   <si>
-    <t>When finished, copy this area into the comment section below table 2c in the FRA platform</t>
-  </si>
-  <si>
     <t>Copy highlighted biomass values into FRA platform table 2c</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>In Sections 1 and 2 you insert data from reporting tables 1b and 2a, and in Section 3  you insert the estimated  percentages of growing stock by combination of FRA forest type and IPCC forest type. Once you are done, copy sections 3 to 8 and paste them in the comment section below table 2c in the FRA platform. Finally, copy the data from Section 9 to table 2c in the platform and data from Section 10 to table 2d in the platform.</t>
+  </si>
+  <si>
+    <t>When finished, copy this area into section Analysis and processing of national data in table 2c in the FRA platform</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1654,7 @@
   <dimension ref="B1:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:L5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1728,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="125" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="125"/>
       <c r="E5" s="125"/>
@@ -2444,7 +2444,7 @@
       <c r="B35" s="34"/>
       <c r="C35" s="36"/>
       <c r="D35" s="49" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
@@ -4982,10 +4982,10 @@
     </row>
     <row r="120" spans="2:14" s="51" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C120" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N120" s="52"/>
     </row>
@@ -5164,10 +5164,10 @@
     </row>
     <row r="128" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C128" s="49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D128" s="76"/>
       <c r="E128" s="76"/>
@@ -5851,7 +5851,7 @@
       <c r="M168" s="76"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="o+oQNtlV04+KJUG005s2Eb3VRI3RhKd1OsOf9KuMM/yTGMGY9s+otfbV2dgiamNGC5nvuCGCUViicd9es8nHtw==" saltValue="VRIFU3I/1JZPq0F6TXwuAg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rQy0DUZSjJYOrNvCOpbqgySCbzdimz5P+1RI81wdhUHglVFDh2QbNU7qZ7N+ODm13lSZmyWP/WuwOVHEjqPnGg==" saltValue="k8k43BBpwTOIycT9DM8tHA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
     <mergeCell ref="C5:L5"/>
     <mergeCell ref="D61:L61"/>

</xml_diff>